<commit_message>
added closed document field
</commit_message>
<xml_diff>
--- a/saybapco/CS_OLD2/000-A-PRI-50002-001-RA-CS REP.xlsx
+++ b/saybapco/CS_OLD2/000-A-PRI-50002-001-RA-CS REP.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\076551C-BAPCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danilo/python/saybapco/saybapco/CS_OLD2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D759852C-E8D2-FB41-B106-9BAD3A1019E9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="000-A-PRI-50002-001-RA-CS" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Subject</t>
   </si>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,48 +622,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -973,28 +974,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="5"/>
-    <col min="4" max="4" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.88671875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="5"/>
-    <col min="7" max="7" width="12.109375" style="5" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="5"/>
+    <col min="4" max="4" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="91.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="5"/>
+    <col min="7" max="7" width="12.1640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="12" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1042,9 +1043,11 @@
       <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1066,9 +1069,11 @@
       <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1090,9 +1095,11 @@
       <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1112,11 +1119,13 @@
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1138,9 +1147,11 @@
       <c r="G6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E16" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>